<commit_message>
Drawing the second cyclist (at the same position)
</commit_message>
<xml_diff>
--- a/Team 5 Cyclist Class Inventory .xlsx
+++ b/Team 5 Cyclist Class Inventory .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc286ffa82667f23/Documentos/Eduardo/Pathway/CSE210_Group/team5_cycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C25F2ABD-98D5-489F-8224-A631C347B046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C25F2ABD-98D5-489F-8224-A631C347B046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AA15A49-6E3F-4B28-BBF9-B74C730FC147}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A635F43B-E867-4C66-9266-A006171BBD5A}"/>
   </bookViews>
@@ -603,7 +603,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,7 +733,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">

</xml_diff>

<commit_message>
Removing food and snake programs
</commit_message>
<xml_diff>
--- a/Team 5 Cyclist Class Inventory .xlsx
+++ b/Team 5 Cyclist Class Inventory .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc286ffa82667f23/Documentos/Eduardo/Pathway/CSE210_Group/team5_cycle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{C25F2ABD-98D5-489F-8224-A631C347B046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AA15A49-6E3F-4B28-BBF9-B74C730FC147}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{C25F2ABD-98D5-489F-8224-A631C347B046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C9EE63B-4CED-4523-9AC1-08D3655A3145}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A635F43B-E867-4C66-9266-A006171BBD5A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>Cast</t>
   </si>
@@ -200,13 +200,38 @@
   </si>
   <si>
     <t>Readme</t>
+  </si>
+  <si>
+    <t>"input", ControlActorsAction(keyboard_service)</t>
+  </si>
+  <si>
+    <r>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>update", MoveActorsAction()</t>
+    </r>
+  </si>
+  <si>
+    <t>"update", HandleCollisionsAction()</t>
+  </si>
+  <si>
+    <t>"output", DrawActorsAction(video_service)</t>
+  </si>
+  <si>
+    <t>Manage the collision</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +261,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -279,13 +315,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,16 +640,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18472D-943B-436A-BAC6-34339E3C1F55}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" customWidth="1"/>
     <col min="4" max="5" width="36.109375" customWidth="1"/>
     <col min="6" max="6" width="26.21875" customWidth="1"/>
   </cols>
@@ -753,6 +793,9 @@
       <c r="C16" t="s">
         <v>26</v>
       </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
       <c r="F16" t="s">
         <v>49</v>
       </c>
@@ -779,79 +822,99 @@
         <v>20</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="C20" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2" t="s">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
         <v>54</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F33" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>